<commit_message>
Accepted only properties display option introduced
</commit_message>
<xml_diff>
--- a/ModelGenApp/Types with a non-unique name.xlsx
+++ b/ModelGenApp/Types with a non-unique name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS\Projects\DocxDocument\ModelGenApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55435454-97DD-4737-B526-4E61F1401A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3151F6E5-B2C7-4602-9472-80A4ADB269A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13410" yWindow="300" windowWidth="14670" windowHeight="14235" xr2:uid="{8FB451F8-01F2-48F8-9909-5E896481FF8A}"/>
+    <workbookView xWindow="9570" yWindow="300" windowWidth="18510" windowHeight="14235" xr2:uid="{8FB451F8-01F2-48F8-9909-5E896481FF8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Oryginalna przestrzeń nazw</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Val</t>
+  </si>
+  <si>
+    <t>On/Off Value</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715BAD7F-604D-488B-82FF-209DFC51ECAF}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
@@ -478,7 +481,7 @@
     <col min="6" max="6" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -504,7 +507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -517,7 +520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -530,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,7 +546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -556,7 +559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -569,7 +572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -582,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
@@ -591,7 +594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
@@ -600,7 +603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
@@ -609,11 +612,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
@@ -624,7 +627,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
@@ -636,8 +639,11 @@
         <v>23</v>
       </c>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
@@ -648,7 +654,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
ConvertTypes phase witched on
</commit_message>
<xml_diff>
--- a/ModelGenApp/Types with a non-unique name.xlsx
+++ b/ModelGenApp/Types with a non-unique name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS\Projects\DocxDocument\ModelGenApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B562D002-520F-42A2-8C9A-3EDFE2BF8648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02154F3-0C17-42A1-BF92-7276E94E0BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD3C08B1-6DE0-4C55-910D-6988886100CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2771" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="524">
   <si>
     <t>Oryginalna przestrzeń nazw</t>
   </si>
@@ -1605,6 +1605,9 @@
   </si>
   <si>
     <t>Xstring</t>
+  </si>
+  <si>
+    <t>true, false, on, off, 0, 1</t>
   </si>
 </sst>
 </file>
@@ -1960,10 +1963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91471DBF-15B8-43F2-BE24-65946792B4AB}">
-  <dimension ref="A1:F1163"/>
+  <dimension ref="A1:G1163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,7 +1979,7 @@
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2010,7 +2013,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2024,7 +2027,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -2038,7 +2041,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2049,8 +2052,11 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2064,7 +2070,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -2076,7 +2082,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2088,7 +2094,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2102,7 +2108,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2114,7 +2120,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2126,7 +2132,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -2138,7 +2144,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2150,7 +2156,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -2164,7 +2170,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2178,7 +2184,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>